<commit_message>
Final graphics tweaks for MEPS submission
</commit_message>
<xml_diff>
--- a/output/rtables/shanpubdata.xlsx
+++ b/output/rtables/shanpubdata.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -395,7 +395,12 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Contrast 66% CI</t>
+          <t>Contrast ratio</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Contrast ratio 95% CI</t>
         </is>
       </c>
     </row>
@@ -429,9 +434,12 @@
           <t>0.29-1.19</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>0.47-1.01</t>
+      <c r="H2">
+        <v>2.48</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>1.42-4.34</t>
         </is>
       </c>
     </row>
@@ -465,9 +473,12 @@
           <t>0.55-1.39</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>0.72-1.22</t>
+      <c r="H3">
+        <v>4.54</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2.3-8.98</t>
         </is>
       </c>
     </row>
@@ -501,9 +512,12 @@
           <t>-0.06-0.51</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>0.06-0.4</t>
+      <c r="H4">
+        <v>1.83</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>0.85-3.93</t>
         </is>
       </c>
     </row>

</xml_diff>